<commit_message>
pengajuan nota, approval audit
</commit_message>
<xml_diff>
--- a/storage/import/user_template_sumo.xlsx
+++ b/storage/import/user_template_sumo.xlsx
@@ -378,10 +378,10 @@
     <t>AUDIT</t>
   </si>
   <si>
-    <t>AUDITOR</t>
-  </si>
-  <si>
     <t>EXECUTOR</t>
+  </si>
+  <si>
+    <t>MEGA</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,7 +1968,7 @@
         <v>117</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -1980,7 +1980,7 @@
         <v>118</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>12</v>

</xml_diff>